<commit_message>
valid credential with excel connect
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aman.aman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aman.aman\Documents\java_selenium_workspace\OpenEmrAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C00AED-0489-43BF-A0FB-B3EF41F13465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61206B9-E15F-4D0A-A4FF-DBC3A0A72970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{874D6DA0-40DE-41A0-8AFE-907CE6D6C0F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{874D6DA0-40DE-41A0-8AFE-907CE6D6C0F8}"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>User Name</t>
   </si>
@@ -71,6 +72,24 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Title</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>OpenEMR</t>
+  </si>
+  <si>
+    <t>physician</t>
+  </si>
+  <si>
+    <t>accountant</t>
   </si>
 </sst>
 </file>
@@ -424,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D1032E-D583-4AD2-8D6B-964E177F5AA3}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,4 +513,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EC8242-2669-4DBB-AE5A-2A3C43EFB3EE}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>